<commit_message>
Made Folder Name Changes
To reflect Git version handling
</commit_message>
<xml_diff>
--- a/Doc_Guide.xlsx
+++ b/Doc_Guide.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mitchel\Dropbox\Jazz IMU\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\Users\Mitchel\Documents\Jazz_IMU\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="2760" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="2760"/>
   </bookViews>
   <sheets>
     <sheet name="Doc List" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
   <si>
     <t>JS</t>
   </si>
@@ -45,12 +45,6 @@
     <t>Prj.</t>
   </si>
   <si>
-    <t>R0</t>
-  </si>
-  <si>
-    <t>Rev</t>
-  </si>
-  <si>
     <t>02</t>
   </si>
   <si>
@@ -69,9 +63,6 @@
     <t>System Document ID:</t>
   </si>
   <si>
-    <t>Revision No.</t>
-  </si>
-  <si>
     <t>System ID Key</t>
   </si>
   <si>
@@ -91,24 +82,6 @@
   </si>
   <si>
     <t>Environmental Simulation Design Document</t>
-  </si>
-  <si>
-    <t>dev</t>
-  </si>
-  <si>
-    <t>Revision Key</t>
-  </si>
-  <si>
-    <t>under development</t>
-  </si>
-  <si>
-    <t>First Release</t>
-  </si>
-  <si>
-    <t>R1, R2, etc..</t>
-  </si>
-  <si>
-    <t>First Revision, 2nd Revision, etc..</t>
   </si>
 </sst>
 </file>
@@ -144,7 +117,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -154,9 +127,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -439,21 +409,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="3.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="44.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="44.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -463,11 +433,8 @@
       <c r="C1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -477,14 +444,11 @@
       <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -492,16 +456,13 @@
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -511,11 +472,8 @@
       <c r="C4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" t="s">
-        <v>21</v>
+      <c r="D4" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -526,10 +484,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -537,24 +495,20 @@
     <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -564,98 +518,57 @@
       <c r="C2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C6" s="4"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="4"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="4"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="4"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="4"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>20</v>
-      </c>
       <c r="C9" s="4"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" s="4"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" s="4"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" s="4"/>
-    </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
+  <mergeCells count="5">
+    <mergeCell ref="A5:C5"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="B9:C9"/>
-    <mergeCell ref="A5:C5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>